<commit_message>
organized and ran data from 20250513
</commit_message>
<xml_diff>
--- a/data/usda-families/metadata/sample_metadata.xlsx
+++ b/data/usda-families/metadata/sample_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/resazurin-assay-development/data/usda-families/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6152610A-133F-2542-B749-96F625115301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4950FA3B-590D-2D47-AD2C-E22FFCE97E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{82B90333-BA24-8845-9D16-9ED0467060EB}"/>
+    <workbookView xWindow="18680" yWindow="760" windowWidth="11560" windowHeight="17760" xr2:uid="{82B90333-BA24-8845-9D16-9ED0467060EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="71">
   <si>
     <t>D1</t>
   </si>
@@ -637,7 +637,7 @@
   <dimension ref="A1:L66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1189,102 +1189,507 @@
       <c r="L31" s="1"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B37" s="1"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B38" s="1"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B39" s="1"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B43" s="1"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B45" s="1"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B46" s="1"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B47" s="1"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="1"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="1"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="1"/>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B54" s="1"/>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="1"/>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="1"/>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B57" s="1"/>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" s="1"/>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B59" s="1"/>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" s="1"/>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>20250513</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20250513</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>20250513</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>20250513</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>20250513</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>20250513</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>20250513</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>20250513</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>20250513</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>20250513</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>20250513</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>20250513</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>20250513</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>20250513</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>20250513</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>20250513</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>20250513</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>20250513</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>20250513</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" t="s">
+        <v>25</v>
+      </c>
+      <c r="E50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>20250513</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>20250513</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D52" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>20250513</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D53" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>20250513</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" t="s">
+        <v>25</v>
+      </c>
+      <c r="E54" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>20250513</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>20250513</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D56" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>20250513</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>20250513</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>20250513</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D59" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>20250513</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>20250513</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B64" s="1"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated resazurin with 5/27 data
</commit_message>
<xml_diff>
--- a/data/usda-families/metadata/sample_metadata.xlsx
+++ b/data/usda-families/metadata/sample_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/resazurin-assay-development/data/usda-families/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EFB742-4C26-9F43-B126-F1C3275B7949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BC497F-39DD-8547-BA41-4D13A836A384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18680" yWindow="760" windowWidth="11560" windowHeight="17760" xr2:uid="{82B90333-BA24-8845-9D16-9ED0467060EB}"/>
+    <workbookView xWindow="9240" yWindow="760" windowWidth="21000" windowHeight="17760" xr2:uid="{82B90333-BA24-8845-9D16-9ED0467060EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="72">
   <si>
     <t>D1</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>remove, dead shell</t>
   </si>
 </sst>
 </file>
@@ -634,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5332F4-46C5-F947-90EB-95CC8225298E}">
-  <dimension ref="A1:L91"/>
+  <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2178,6 +2181,504 @@
         <v>64</v>
       </c>
     </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>20250527</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D92" t="s">
+        <v>25</v>
+      </c>
+      <c r="E92" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>20250527</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D93" t="s">
+        <v>25</v>
+      </c>
+      <c r="E93" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>20250527</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D94" t="s">
+        <v>25</v>
+      </c>
+      <c r="E94" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>20250527</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D95" t="s">
+        <v>25</v>
+      </c>
+      <c r="E95" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>20250527</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D96" t="s">
+        <v>25</v>
+      </c>
+      <c r="E96" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>20250527</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D97" t="s">
+        <v>25</v>
+      </c>
+      <c r="E97" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>20250527</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D98" t="s">
+        <v>25</v>
+      </c>
+      <c r="E98" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>20250527</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D99" t="s">
+        <v>25</v>
+      </c>
+      <c r="E99" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>20250527</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D100" t="s">
+        <v>25</v>
+      </c>
+      <c r="E100" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>20250527</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D101" t="s">
+        <v>25</v>
+      </c>
+      <c r="E101" t="s">
+        <v>67</v>
+      </c>
+      <c r="F101" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>20250527</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D102" t="s">
+        <v>25</v>
+      </c>
+      <c r="E102" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>20250527</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D103" t="s">
+        <v>25</v>
+      </c>
+      <c r="E103" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>20250527</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D104" t="s">
+        <v>25</v>
+      </c>
+      <c r="E104" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>20250527</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D105" t="s">
+        <v>25</v>
+      </c>
+      <c r="E105" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>20250527</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D106" t="s">
+        <v>25</v>
+      </c>
+      <c r="E106" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>20250527</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D107" t="s">
+        <v>25</v>
+      </c>
+      <c r="E107" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>20250527</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D108" t="s">
+        <v>25</v>
+      </c>
+      <c r="E108" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>20250527</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D109" t="s">
+        <v>25</v>
+      </c>
+      <c r="E109" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>20250527</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D110" t="s">
+        <v>25</v>
+      </c>
+      <c r="E110" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>20250527</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D111" t="s">
+        <v>25</v>
+      </c>
+      <c r="E111" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>20250527</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D112" t="s">
+        <v>25</v>
+      </c>
+      <c r="E112" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>20250527</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D113" t="s">
+        <v>25</v>
+      </c>
+      <c r="E113" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>20250527</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D114" t="s">
+        <v>25</v>
+      </c>
+      <c r="E114" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>20250527</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D115" t="s">
+        <v>25</v>
+      </c>
+      <c r="E115" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>20250527</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D116" t="s">
+        <v>25</v>
+      </c>
+      <c r="E116" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>20250527</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D117" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>20250527</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D118" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>20250527</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D119" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>20250527</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D120" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>20250527</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D121" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran final round of usda families resazurin data
</commit_message>
<xml_diff>
--- a/data/usda-families/metadata/sample_metadata.xlsx
+++ b/data/usda-families/metadata/sample_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashuffmyer/MyProjects/oysters/resazurin-assay-development/data/usda-families/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64A9EEF-5A2B-1B4A-806A-48F7A30ECCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DE1150-FA03-E441-9A79-D9BCA66B134E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9240" yWindow="760" windowWidth="21000" windowHeight="17760" xr2:uid="{82B90333-BA24-8845-9D16-9ED0467060EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="73">
   <si>
     <t>D1</t>
   </si>
@@ -640,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5332F4-46C5-F947-90EB-95CC8225298E}">
-  <dimension ref="A1:L151"/>
+  <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="F135" sqref="F135"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="B178" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3183,6 +3183,501 @@
         <v>64</v>
       </c>
     </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>20250610</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D152" t="s">
+        <v>25</v>
+      </c>
+      <c r="E152" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>20250610</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D153" t="s">
+        <v>25</v>
+      </c>
+      <c r="E153" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>20250610</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D154" t="s">
+        <v>25</v>
+      </c>
+      <c r="E154" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>20250610</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D155" t="s">
+        <v>25</v>
+      </c>
+      <c r="E155" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>20250610</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D156" t="s">
+        <v>25</v>
+      </c>
+      <c r="E156" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>20250610</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D157" t="s">
+        <v>25</v>
+      </c>
+      <c r="E157" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>20250610</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D158" t="s">
+        <v>25</v>
+      </c>
+      <c r="E158" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>20250610</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D159" t="s">
+        <v>25</v>
+      </c>
+      <c r="E159" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>20250610</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D160" t="s">
+        <v>25</v>
+      </c>
+      <c r="E160" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>20250610</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D161" t="s">
+        <v>25</v>
+      </c>
+      <c r="E161" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>20250610</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D162" t="s">
+        <v>25</v>
+      </c>
+      <c r="E162" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>20250610</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D163" t="s">
+        <v>25</v>
+      </c>
+      <c r="E163" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>20250610</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D164" t="s">
+        <v>25</v>
+      </c>
+      <c r="E164" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>20250610</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D165" t="s">
+        <v>25</v>
+      </c>
+      <c r="E165" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>20250610</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D166" t="s">
+        <v>25</v>
+      </c>
+      <c r="E166" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>20250610</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D167" t="s">
+        <v>25</v>
+      </c>
+      <c r="E167" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>20250610</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D168" t="s">
+        <v>25</v>
+      </c>
+      <c r="E168" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>20250610</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D169" t="s">
+        <v>25</v>
+      </c>
+      <c r="E169" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>20250610</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D170" t="s">
+        <v>25</v>
+      </c>
+      <c r="E170" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>20250610</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D171" t="s">
+        <v>25</v>
+      </c>
+      <c r="E171" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>20250610</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D172" t="s">
+        <v>25</v>
+      </c>
+      <c r="E172" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>20250610</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D173" t="s">
+        <v>25</v>
+      </c>
+      <c r="E173" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>20250610</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D174" t="s">
+        <v>25</v>
+      </c>
+      <c r="E174" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>20250610</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D175" t="s">
+        <v>25</v>
+      </c>
+      <c r="E175" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>20250610</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D176" t="s">
+        <v>25</v>
+      </c>
+      <c r="E176" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>20250610</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D177" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>20250610</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D178" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>20250610</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D179" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>20250610</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D180" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>20250610</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D181" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>